<commit_message>
Section 1 Visualization Update
</commit_message>
<xml_diff>
--- a/Data/Social_Data/Crime_Against_Women/crime_against_women(1998-2015).xlsx
+++ b/Data/Social_Data/Crime_Against_Women/crime_against_women(1998-2015).xlsx
@@ -5,14 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ambika/Documents/Final_Project_V2/Social_Data/Crime_Against_Women/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ambika/Documents/Final_Project_V2/Data/Social_Data/Crime_Against_Women/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="1680" windowWidth="27760" windowHeight="15300" tabRatio="500"/>
+    <workbookView xWindow="1040" yWindow="1680" windowWidth="27760" windowHeight="15300" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
   <si>
     <t>Year</t>
   </si>
@@ -382,8 +383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1170,4 +1171,786 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1998</v>
+      </c>
+      <c r="C1">
+        <v>1999</v>
+      </c>
+      <c r="D1">
+        <v>2000</v>
+      </c>
+      <c r="E1">
+        <v>2001</v>
+      </c>
+      <c r="F1">
+        <v>2002</v>
+      </c>
+      <c r="G1">
+        <v>2003</v>
+      </c>
+      <c r="H1">
+        <v>2004</v>
+      </c>
+      <c r="I1">
+        <v>2005</v>
+      </c>
+      <c r="J1">
+        <v>2006</v>
+      </c>
+      <c r="K1">
+        <v>2007</v>
+      </c>
+      <c r="L1">
+        <v>2008</v>
+      </c>
+      <c r="M1">
+        <v>2009</v>
+      </c>
+      <c r="N1">
+        <v>2010</v>
+      </c>
+      <c r="O1">
+        <v>2011</v>
+      </c>
+      <c r="P1">
+        <v>2012</v>
+      </c>
+      <c r="Q1">
+        <v>2013</v>
+      </c>
+      <c r="R1">
+        <v>2014</v>
+      </c>
+      <c r="S1">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>368</v>
+      </c>
+      <c r="C2">
+        <v>331</v>
+      </c>
+      <c r="D2">
+        <v>330</v>
+      </c>
+      <c r="E2">
+        <v>286</v>
+      </c>
+      <c r="F2">
+        <v>267</v>
+      </c>
+      <c r="G2">
+        <v>236</v>
+      </c>
+      <c r="H2">
+        <v>339</v>
+      </c>
+      <c r="I2">
+        <v>324</v>
+      </c>
+      <c r="J2">
+        <v>354</v>
+      </c>
+      <c r="K2">
+        <v>316</v>
+      </c>
+      <c r="L2">
+        <v>374</v>
+      </c>
+      <c r="M2">
+        <v>433</v>
+      </c>
+      <c r="N2">
+        <v>408</v>
+      </c>
+      <c r="O2">
+        <v>439</v>
+      </c>
+      <c r="P2">
+        <v>473</v>
+      </c>
+      <c r="Q2">
+        <v>732</v>
+      </c>
+      <c r="R2">
+        <v>841</v>
+      </c>
+      <c r="S2">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1182</v>
+      </c>
+      <c r="C3">
+        <v>1074</v>
+      </c>
+      <c r="D3">
+        <v>868</v>
+      </c>
+      <c r="E3">
+        <v>857</v>
+      </c>
+      <c r="F3">
+        <v>807</v>
+      </c>
+      <c r="G3">
+        <v>859</v>
+      </c>
+      <c r="H3">
+        <v>905</v>
+      </c>
+      <c r="I3">
+        <v>916</v>
+      </c>
+      <c r="J3">
+        <v>945</v>
+      </c>
+      <c r="K3">
+        <v>1089</v>
+      </c>
+      <c r="L3">
+        <v>1119</v>
+      </c>
+      <c r="M3">
+        <v>1162</v>
+      </c>
+      <c r="N3">
+        <v>1290</v>
+      </c>
+      <c r="O3">
+        <v>1442</v>
+      </c>
+      <c r="P3">
+        <v>1527</v>
+      </c>
+      <c r="Q3">
+        <v>2230</v>
+      </c>
+      <c r="R3">
+        <v>2187</v>
+      </c>
+      <c r="S3">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>90</v>
+      </c>
+      <c r="C4">
+        <v>94</v>
+      </c>
+      <c r="D4">
+        <v>93</v>
+      </c>
+      <c r="E4">
+        <v>67</v>
+      </c>
+      <c r="F4">
+        <v>62</v>
+      </c>
+      <c r="G4">
+        <v>54</v>
+      </c>
+      <c r="H4">
+        <v>58</v>
+      </c>
+      <c r="I4">
+        <v>48</v>
+      </c>
+      <c r="J4">
+        <v>50</v>
+      </c>
+      <c r="K4">
+        <v>42</v>
+      </c>
+      <c r="L4">
+        <v>27</v>
+      </c>
+      <c r="M4">
+        <v>24</v>
+      </c>
+      <c r="N4">
+        <v>19</v>
+      </c>
+      <c r="O4">
+        <v>30</v>
+      </c>
+      <c r="P4">
+        <v>21</v>
+      </c>
+      <c r="Q4">
+        <v>29</v>
+      </c>
+      <c r="R4">
+        <v>23</v>
+      </c>
+      <c r="S4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>3602</v>
+      </c>
+      <c r="C5">
+        <v>3886</v>
+      </c>
+      <c r="D5">
+        <v>3739</v>
+      </c>
+      <c r="E5">
+        <v>3667</v>
+      </c>
+      <c r="F5">
+        <v>3321</v>
+      </c>
+      <c r="G5">
+        <v>3684</v>
+      </c>
+      <c r="H5">
+        <v>3955</v>
+      </c>
+      <c r="I5">
+        <v>4090</v>
+      </c>
+      <c r="J5">
+        <v>4977</v>
+      </c>
+      <c r="K5">
+        <v>5827</v>
+      </c>
+      <c r="L5">
+        <v>6094</v>
+      </c>
+      <c r="M5">
+        <v>5506</v>
+      </c>
+      <c r="N5">
+        <v>5600</v>
+      </c>
+      <c r="O5">
+        <v>6052</v>
+      </c>
+      <c r="P5">
+        <v>6658</v>
+      </c>
+      <c r="Q5">
+        <v>7812</v>
+      </c>
+      <c r="R5">
+        <v>5991</v>
+      </c>
+      <c r="S5">
+        <v>4133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1210</v>
+      </c>
+      <c r="C6">
+        <v>1083</v>
+      </c>
+      <c r="D6">
+        <v>944</v>
+      </c>
+      <c r="E6">
+        <v>756</v>
+      </c>
+      <c r="F6">
+        <v>750</v>
+      </c>
+      <c r="G6">
+        <v>722</v>
+      </c>
+      <c r="H6">
+        <v>757</v>
+      </c>
+      <c r="I6">
+        <v>802</v>
+      </c>
+      <c r="J6">
+        <v>736</v>
+      </c>
+      <c r="K6">
+        <v>822</v>
+      </c>
+      <c r="L6">
+        <v>828</v>
+      </c>
+      <c r="M6">
+        <v>727</v>
+      </c>
+      <c r="N6">
+        <v>668</v>
+      </c>
+      <c r="O6">
+        <v>685</v>
+      </c>
+      <c r="P6">
+        <v>745</v>
+      </c>
+      <c r="Q6">
+        <v>1243</v>
+      </c>
+      <c r="R6">
+        <v>1352</v>
+      </c>
+      <c r="S6">
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>139</v>
+      </c>
+      <c r="C7">
+        <v>172</v>
+      </c>
+      <c r="D7">
+        <v>119</v>
+      </c>
+      <c r="E7">
+        <v>111</v>
+      </c>
+      <c r="F7">
+        <v>104</v>
+      </c>
+      <c r="G7">
+        <v>92</v>
+      </c>
+      <c r="H7">
+        <v>164</v>
+      </c>
+      <c r="I7">
+        <v>104</v>
+      </c>
+      <c r="J7">
+        <v>138</v>
+      </c>
+      <c r="K7">
+        <v>120</v>
+      </c>
+      <c r="L7">
+        <v>122</v>
+      </c>
+      <c r="M7">
+        <v>114</v>
+      </c>
+      <c r="N7">
+        <v>110</v>
+      </c>
+      <c r="O7">
+        <v>93</v>
+      </c>
+      <c r="P7">
+        <v>93</v>
+      </c>
+      <c r="Q7">
+        <v>77</v>
+      </c>
+      <c r="R7">
+        <v>173</v>
+      </c>
+      <c r="S7">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>57</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>40</v>
+      </c>
+      <c r="D10">
+        <v>47</v>
+      </c>
+      <c r="E10">
+        <v>61</v>
+      </c>
+      <c r="F10">
+        <v>57</v>
+      </c>
+      <c r="G10">
+        <v>74</v>
+      </c>
+      <c r="H10">
+        <v>33</v>
+      </c>
+      <c r="I10">
+        <v>59</v>
+      </c>
+      <c r="J10">
+        <v>78</v>
+      </c>
+      <c r="K10">
+        <v>44</v>
+      </c>
+      <c r="L10">
+        <v>52</v>
+      </c>
+      <c r="M10">
+        <v>41</v>
+      </c>
+      <c r="N10">
+        <v>46</v>
+      </c>
+      <c r="O10">
+        <v>46</v>
+      </c>
+      <c r="P10">
+        <v>44</v>
+      </c>
+      <c r="Q10">
+        <v>76</v>
+      </c>
+      <c r="R10">
+        <v>45</v>
+      </c>
+      <c r="S10">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <v>14</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>13</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>84</v>
+      </c>
+      <c r="R12">
+        <v>53</v>
+      </c>
+      <c r="S12">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>6658</v>
+      </c>
+      <c r="C13">
+        <v>6694</v>
+      </c>
+      <c r="D13">
+        <v>6140</v>
+      </c>
+      <c r="E13">
+        <v>5805</v>
+      </c>
+      <c r="F13">
+        <v>5373</v>
+      </c>
+      <c r="G13">
+        <v>5735</v>
+      </c>
+      <c r="H13">
+        <v>6211</v>
+      </c>
+      <c r="I13">
+        <v>6343</v>
+      </c>
+      <c r="J13">
+        <v>7279</v>
+      </c>
+      <c r="K13">
+        <v>8260</v>
+      </c>
+      <c r="L13">
+        <v>8616</v>
+      </c>
+      <c r="M13">
+        <v>8009</v>
+      </c>
+      <c r="N13">
+        <v>8148</v>
+      </c>
+      <c r="O13">
+        <v>8815</v>
+      </c>
+      <c r="P13">
+        <v>9561</v>
+      </c>
+      <c r="Q13">
+        <v>12283</v>
+      </c>
+      <c r="R13">
+        <v>10665</v>
+      </c>
+      <c r="S13">
+        <v>7525</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>